<commit_message>
upload validator and update | checkin | checkout | set usable | distribute | search by roomNo | search by studentNo
</commit_message>
<xml_diff>
--- a/DormManagement/Server/upload/bedInfo.xlsx
+++ b/DormManagement/Server/upload/bedInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\TinyHeart\DormManagement\Server\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -61,23 +61,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>E1224</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>女</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>已入住</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>罗琳</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E1224</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>女</t>
   </si>
   <si>
     <t>空床</t>
@@ -430,7 +419,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -473,46 +462,37 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="2">
+      <c r="B2" s="2">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
-        <v>5214</v>
-      </c>
-      <c r="D2" s="2">
-        <v>3</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1601210652</v>
-      </c>
-      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
       <c r="B3" s="2">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
+      <c r="C3" s="2">
+        <v>1224</v>
       </c>
       <c r="D3" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -533,6 +513,5 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>